<commit_message>
alterado os tempos de jogo
</commit_message>
<xml_diff>
--- a/Acompanhamento_Mensal_Template.xlsx
+++ b/Acompanhamento_Mensal_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\NetBeansProjects\Monthly-Accounting-followUp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E43D66-DB1E-46FB-B351-342D03E42E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1F6419-2361-4400-952C-CEAF8E04625D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D542A08B-5777-4467-ABBE-F253DBDF7F15}"/>
+    <workbookView xWindow="4872" yWindow="1236" windowWidth="17280" windowHeight="9420" xr2:uid="{D542A08B-5777-4467-ABBE-F253DBDF7F15}"/>
   </bookViews>
   <sheets>
     <sheet name="Acompanhamento" sheetId="1" r:id="rId1"/>
@@ -250,33 +250,23 @@
     <xf numFmtId="4" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -308,97 +298,9 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1A2911"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF1A2911"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFF8F8F8"/>
       <color rgb="FFFF9393"/>
@@ -422,10 +324,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="9CA5BC"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="161A21"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -717,7 +619,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,108 +639,108 @@
       </c>
       <c r="C1" s="3" t="str">
         <f xml:space="preserve"> "Jan " &amp; Ano-1</f>
-        <v>Jan 2020</v>
+        <v>Jan 2019</v>
       </c>
       <c r="D1" s="3" t="str">
         <f xml:space="preserve"> "Jan " &amp; Ano</f>
-        <v>Jan 2021</v>
+        <v>Jan 2020</v>
       </c>
       <c r="E1" s="3" t="str">
         <f xml:space="preserve"> "Fev " &amp; Ano-1</f>
-        <v>Fev 2020</v>
+        <v>Fev 2019</v>
       </c>
       <c r="F1" s="3" t="str">
         <f xml:space="preserve"> "Fev " &amp; Ano</f>
-        <v>Fev 2021</v>
+        <v>Fev 2020</v>
       </c>
       <c r="G1" s="3" t="str">
         <f xml:space="preserve"> "Mar " &amp; Ano-1</f>
-        <v>Mar 2020</v>
+        <v>Mar 2019</v>
       </c>
       <c r="H1" s="3" t="str">
         <f xml:space="preserve"> "Mar " &amp; Ano</f>
-        <v>Mar 2021</v>
+        <v>Mar 2020</v>
       </c>
       <c r="I1" s="3" t="str">
         <f xml:space="preserve"> "Abr " &amp; Ano-1</f>
-        <v>Abr 2020</v>
+        <v>Abr 2019</v>
       </c>
       <c r="J1" s="3" t="str">
         <f xml:space="preserve"> "Abr " &amp; Ano</f>
-        <v>Abr 2021</v>
+        <v>Abr 2020</v>
       </c>
       <c r="K1" s="3" t="str">
         <f xml:space="preserve"> "Mai " &amp; Ano-1</f>
-        <v>Mai 2020</v>
+        <v>Mai 2019</v>
       </c>
       <c r="L1" s="3" t="str">
         <f xml:space="preserve"> "Mai " &amp; Ano</f>
-        <v>Mai 2021</v>
+        <v>Mai 2020</v>
       </c>
       <c r="M1" s="3" t="str">
         <f xml:space="preserve"> "Jun " &amp; Ano-1</f>
-        <v>Jun 2020</v>
+        <v>Jun 2019</v>
       </c>
       <c r="N1" s="3" t="str">
         <f xml:space="preserve"> "Jun " &amp; Ano</f>
-        <v>Jun 2021</v>
+        <v>Jun 2020</v>
       </c>
       <c r="O1" s="3" t="str">
         <f xml:space="preserve"> "Jul " &amp; Ano-1</f>
-        <v>Jul 2020</v>
+        <v>Jul 2019</v>
       </c>
       <c r="P1" s="3" t="str">
         <f xml:space="preserve"> "Jul " &amp; Ano</f>
-        <v>Jul 2021</v>
+        <v>Jul 2020</v>
       </c>
       <c r="Q1" s="3" t="str">
         <f xml:space="preserve"> "Ago " &amp; Ano-1</f>
-        <v>Ago 2020</v>
+        <v>Ago 2019</v>
       </c>
       <c r="R1" s="3" t="str">
         <f xml:space="preserve"> "Ago " &amp; Ano</f>
-        <v>Ago 2021</v>
+        <v>Ago 2020</v>
       </c>
       <c r="S1" s="3" t="str">
         <f xml:space="preserve"> "Set " &amp; Ano-1</f>
-        <v>Set 2020</v>
+        <v>Set 2019</v>
       </c>
       <c r="T1" s="3" t="str">
         <f xml:space="preserve"> "Set " &amp; Ano</f>
-        <v>Set 2021</v>
+        <v>Set 2020</v>
       </c>
       <c r="U1" s="3" t="str">
         <f xml:space="preserve"> "Out " &amp; Ano-1</f>
-        <v>Out 2020</v>
+        <v>Out 2019</v>
       </c>
       <c r="V1" s="3" t="str">
         <f xml:space="preserve"> "Out " &amp; Ano</f>
-        <v>Out 2021</v>
+        <v>Out 2020</v>
       </c>
       <c r="W1" s="3" t="str">
         <f xml:space="preserve"> "Nov " &amp; Ano-1</f>
-        <v>Nov 2020</v>
+        <v>Nov 2019</v>
       </c>
       <c r="X1" s="3" t="str">
         <f xml:space="preserve"> "Nov " &amp; Ano</f>
-        <v>Nov 2021</v>
+        <v>Nov 2020</v>
       </c>
       <c r="Y1" s="3" t="str">
         <f xml:space="preserve"> "Dez " &amp; Ano-1</f>
-        <v>Dez 2020</v>
+        <v>Dez 2019</v>
       </c>
       <c r="Z1" s="3" t="str">
         <f xml:space="preserve"> "Dez " &amp; Ano</f>
-        <v>Dez 2021</v>
+        <v>Dez 2020</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -850,16 +752,16 @@
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:26" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
@@ -878,22 +780,22 @@
       <c r="A13" s="1"/>
     </row>
     <row r="1048576" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D1048576" s="16"/>
+      <c r="D1048576" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A6:A7"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(D2&gt;0,(D2-C2)&gt;100)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:Z1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>